<commit_message>
using setting written in the worksheet itself
</commit_message>
<xml_diff>
--- a/test-input-file/input.xlsx
+++ b/test-input-file/input.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="28">
   <si>
     <t>MMF:</t>
   </si>
@@ -132,10 +132,19 @@
     <t>Titre de la US de vrai 1 de l'excel!!!</t>
   </si>
   <si>
-    <t>Cards per Page</t>
-  </si>
-  <si>
     <t>Num Setting Rows</t>
+  </si>
+  <si>
+    <t>Lines of cards per Page</t>
+  </si>
+  <si>
+    <t>Cards per row</t>
+  </si>
+  <si>
+    <t>Card height in rows</t>
+  </si>
+  <si>
+    <t>Card width in columns</t>
   </si>
 </sst>
 </file>
@@ -255,8 +264,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -285,13 +312,31 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="25">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1647,10 +1692,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1660,81 +1705,105 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1"/>
-    <row r="4" spans="1:6" ht="52" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6" ht="20" thickTop="1" thickBot="1">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:6" ht="69" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" thickBot="1"/>
+    <row r="7" spans="1:6" ht="52" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A7" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" ht="20" thickTop="1" thickBot="1">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" ht="69" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" ht="20" thickTop="1" thickBot="1">
-      <c r="A7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" ht="15" thickTop="1"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" ht="20" thickTop="1" thickBot="1">
+      <c r="A10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" ht="15" thickTop="1"/>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="E7:F7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="E8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
US cards are now loaded in a different way: the items of the header row must match the list of attributes of the USCard. Also started some work on Features, but nothing really working yet
</commit_message>
<xml_diff>
--- a/test-input-file/input.xlsx
+++ b/test-input-file/input.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Story Map Data" sheetId="4" r:id="rId1"/>
+    <sheet name="Feature Data" sheetId="4" r:id="rId1"/>
     <sheet name="US Data" sheetId="2" r:id="rId2"/>
     <sheet name="US Template" sheetId="1" r:id="rId3"/>
   </sheets>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="37">
   <si>
     <t>MMF:</t>
   </si>
@@ -149,6 +149,30 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>US_ID</t>
+  </si>
+  <si>
+    <t>Feature 1</t>
+  </si>
+  <si>
+    <t>Feature 1 TITLE</t>
+  </si>
+  <si>
+    <t>Feature 2</t>
+  </si>
+  <si>
+    <t>Feature 2 TITLE</t>
+  </si>
+  <si>
+    <t>Feature 3</t>
+  </si>
+  <si>
+    <t>Feature 3 TITLE</t>
+  </si>
+  <si>
+    <t>FEATURE_ID</t>
   </si>
 </sst>
 </file>
@@ -268,8 +292,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -316,7 +346,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="31">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -329,6 +359,9 @@
     <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -341,6 +374,9 @@
     <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -731,13 +767,226 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -750,7 +999,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>

</xml_diff>